<commit_message>
Update 229 first anniversary
</commit_message>
<xml_diff>
--- a/data/Dialog/dialog.xlsx
+++ b/data/Dialog/dialog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="593">
   <si>
     <t>id</t>
   </si>
@@ -1869,6 +1869,96 @@
 Yes #race, you're standing in front of an exile who has lived more than 1000 years.</t>
   </si>
   <si>
+    <t>namamani</t>
+  </si>
+  <si>
+    <t>Đây là nơi nào?</t>
+  </si>
+  <si>
+    <t>なんだこの場所は？</t>
+  </si>
+  <si>
+    <t>What is this place?</t>
+  </si>
+  <si>
+    <t>namamani2</t>
+  </si>
+  <si>
+    <t>Lạ thật... Tôi không thể nhớ bất cứ điều gì.</t>
+  </si>
+  <si>
+    <t>おかしい、何も思い出せない。</t>
+  </si>
+  <si>
+    <t>Strange... I can't remember anything.</t>
+  </si>
+  <si>
+    <t>keeper_garden</t>
+  </si>
+  <si>
+    <t>"Tanelorn? À, ta có nghe ai đó gọi nơi này bằng cái tên đó rồi." 
+"Sao thế? Ngươi cũng muốn được ta cưng chiều à?" 
+"Thời gian ở đây chẳng có ý nghĩa gì sất." 
+"Ồ? Ngươi là lữ khách, hay kẻ lạc lối, hay là một tên ngốc lang thang đến đây mà còn không biết đây là đâu?" 
+"Cứ đi đâu tùy ngươi. Dù đi đâu thì cũng chỉ có cảnh vật y hệt vậy thôi." 
+"Muwohoho... lại còn chào hỏi ta, đúng là một kẻ lễ phép."</t>
+  </si>
+  <si>
+    <t>タネローン？ ああ、誰かが庭をそう呼ぶのを聞いたことがあるな。
+なんじゃ、ぬしもわっちに可愛がられたい口か？ 
+時などここでは何の意味も持たぬのじゃ。
+ほう、旅人か、迷子か、それとも、 ここがどこかも知らずに歩いてきた愚か者か。
+好きに歩け。どこへ行っても、同じ景色じゃ。 
+フホホホ、わっちに挨拶とは律儀なやつじゃ。</t>
+  </si>
+  <si>
+    <t>Tanelorn? Ah, I’ve heard someone call this place by that name before.
+What is it? Do you wish to be doted on by me as well?
+Time holds no meaning here.
+Oh? A traveler, a lost one, or perhaps just a fool wandering without knowing where you’ve come?
+Walk wherever you please. Every path leads to the same view.
+Muwohoho... how courteous of you to greet me, mortal.</t>
+  </si>
+  <si>
+    <t>erishe</t>
+  </si>
+  <si>
+    <t>"Hì hì, anh ơi, anh đi đâu rồi?" 
+"Chào bạn, lữ khách. Xin cứ tự nhiên nghỉ ngơi ở đây." 
+"Nơi này thật là bình yên. Ở đây cứ như là khiến người ta quên mất cả thời gian vậy..." 
+"Tôi bị lạc anh trai trên đường đi xem kịch. Không biết đã có chuyện gì xảy ra nhỉ?" 
+"Cả anh trai tôi và tôi đều không thực sự hứng thú với kịch nghệ. Nhưng ở Zanan, đó được coi là một phần tu dưỡng của quý tộc." 
+"Bạn có biết không...? Ở Altheheit có tiên tộc đấy." 
+"Anh ấy trông vậy thôi, chứ không có tôi là vô dụng lắm, hì hì." 
+"Anh Loyter, hình như có lần ảnh ném đá ở phòng hòa nhạc nên bị cấm cửa luôn thì phải." 
+"Mỗi khi tôi mang quà đến, anh Loyter lại đỏ mặt như một cậu con trai mới lớn vậy đó." 
+"Loytel...? Không, tôi không nghĩ vậy, nhưng tôi có biết anh Loyter..."</t>
+  </si>
+  <si>
+    <t>ふふ、兄さん、どこにいったの？
+こんにちは、旅の人。ゆっくりしていってください。
+とても平和な場所です。ここにいると、まるで時間を忘れてしまうようで…
+お芝居を見に行く途中で、兄さんとはぐれてしまって。何が起こったのでしょう？
+兄さんも私も、お芝居にはあまり興味はないんです。でも、ザナンでは貴族のたしなみですから。
+知っていましたか…？ アルティハイトには妖精がいるんですよ？
+ああ見えても、兄さんは私がいないとだらしないんですよ、ふふ。
+ロイターさんは、演奏会場で石を投げて、出入り禁止になったことがあるようですね。
+差し入れを持っていくと、ロイターさんったら、いまだに少年みたいに照れるんですよ。
+ロイテル…？ いえ、ロイターさんなら知ってますけど…</t>
+  </si>
+  <si>
+    <t>Hehe, brother, where did you go?
+Hello, traveler. Please, take your time and rest here.
+This is such a peaceful place. Being here almost makes you forget about time itself...
+I got separated from my brother on the way to the play. I wonder what happened?
+Neither of us is really interested in theater, but in Zanan, it’s considered part of a noble’s education.
+Did you know? …There are fairies in Altheheit, you know.
+Even though he doesn’t look it, my brother is hopeless without me, hehe.
+Loyter once threw a stone at a concert hall and got himself banned from entering.
+Whenever I bring Loyter a little gift, he still blushes like a boy.
+Loytel...? I don’t think so, though I do know Loyter.</t>
+  </si>
+  <si>
     <t>larnneire</t>
   </si>
   <si>
@@ -3036,14 +3126,14 @@
       <name val="Times New Roman"/>
     </font>
     <font>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="MS PGothic"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -3077,7 +3167,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3097,16 +3187,19 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3342,7 +3435,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="19.14"/>
-    <col customWidth="1" min="2" max="2" width="10.43"/>
+    <col customWidth="1" min="2" max="2" width="54.0"/>
     <col customWidth="1" min="3" max="3" width="95.57"/>
     <col customWidth="1" min="4" max="4" width="86.29"/>
     <col customWidth="1" min="5" max="6" width="14.43"/>
@@ -9994,7 +10087,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="13.57"/>
-    <col customWidth="1" min="2" max="2" width="44.29"/>
+    <col customWidth="1" min="2" max="2" width="10.71"/>
     <col customWidth="1" min="3" max="3" width="117.57"/>
     <col customWidth="1" min="4" max="4" width="122.71"/>
     <col customWidth="1" min="5" max="26" width="11.57"/>
@@ -16185,7 +16278,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="15.71"/>
-    <col customWidth="1" min="2" max="2" width="38.71"/>
+    <col customWidth="1" min="2" max="2" width="13.57"/>
     <col customWidth="1" min="3" max="3" width="109.14"/>
     <col customWidth="1" min="4" max="4" width="123.0"/>
     <col customWidth="1" min="5" max="26" width="11.57"/>
@@ -22327,7 +22420,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="14.57"/>
-    <col customWidth="1" min="2" max="2" width="34.71"/>
+    <col customWidth="1" min="2" max="2" width="39.0"/>
     <col customWidth="1" min="3" max="3" width="111.0"/>
     <col customWidth="1" min="4" max="4" width="100.57"/>
     <col customWidth="1" min="5" max="26" width="11.57"/>
@@ -22369,13 +22462,13 @@
       <c r="A5" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="9" t="s">
         <v>423</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="1" t="s">
         <v>425</v>
       </c>
     </row>
@@ -22383,21 +22476,21 @@
       <c r="A6" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="9" t="s">
         <v>427</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="10" t="s">
         <v>430</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="9" t="s">
         <v>431</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -22411,7 +22504,7 @@
       <c r="A8" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="11" t="s">
         <v>435</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -22495,7 +22588,7 @@
       <c r="A14" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>459</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -22515,7 +22608,7 @@
       <c r="C15" s="4" t="s">
         <v>464</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="4" t="s">
         <v>465</v>
       </c>
     </row>
@@ -22551,7 +22644,7 @@
       <c r="A18" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>475</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -22571,7 +22664,7 @@
       <c r="C19" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="1" t="s">
         <v>481</v>
       </c>
     </row>
@@ -22627,7 +22720,7 @@
       <c r="C23" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="4" t="s">
         <v>497</v>
       </c>
     </row>
@@ -22652,10 +22745,10 @@
       <c r="B25" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="4" t="s">
         <v>505</v>
       </c>
     </row>
@@ -22674,7 +22767,7 @@
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="1" t="s">
         <v>510</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -22683,88 +22776,88 @@
       <c r="C27" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>253</v>
+      <c r="D27" s="12" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="10" t="s">
-        <v>513</v>
+      <c r="A28" s="1" t="s">
+        <v>514</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="C28" s="11" t="s">
         <v>515</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="C28" s="4" t="s">
         <v>516</v>
       </c>
+      <c r="D28" s="4" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="10" t="s">
-        <v>517</v>
+      <c r="A29" s="1" t="s">
+        <v>518</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>519</v>
-      </c>
-      <c r="D29" s="4" t="s">
         <v>520</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>523</v>
-      </c>
-      <c r="D30" s="5" t="s">
         <v>524</v>
       </c>
+      <c r="D30" s="4" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="4" t="s">
-        <v>525</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="A31" s="10" t="s">
         <v>526</v>
       </c>
+      <c r="B31" s="3" t="s">
+        <v>527</v>
+      </c>
       <c r="C31" s="4" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>528</v>
+        <v>253</v>
       </c>
     </row>
     <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="10" t="s">
         <v>529</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="13" t="s">
         <v>531</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="1" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="10" t="s">
         <v>533</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="14" t="s">
         <v>535</v>
       </c>
       <c r="D33" s="4" t="s">
@@ -22772,16 +22865,16 @@
       </c>
     </row>
     <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="5" t="s">
         <v>540</v>
       </c>
     </row>
@@ -22800,10 +22893,10 @@
       </c>
     </row>
     <row r="36" ht="12.75" customHeight="1">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="1" t="s">
         <v>546</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -22814,10 +22907,10 @@
       </c>
     </row>
     <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="1" t="s">
         <v>550</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -22828,13 +22921,13 @@
       </c>
     </row>
     <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="1" t="s">
         <v>555</v>
       </c>
       <c r="D38" s="4" t="s">
@@ -22842,10 +22935,10 @@
       </c>
     </row>
     <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="1" t="s">
         <v>558</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -22856,7 +22949,7 @@
       </c>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="1" t="s">
         <v>561</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -22870,10 +22963,10 @@
       </c>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="3" t="s">
         <v>566</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -22887,7 +22980,7 @@
       <c r="A42" s="10" t="s">
         <v>569</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="3" t="s">
         <v>570</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -22912,28 +23005,60 @@
       </c>
     </row>
     <row r="44" ht="12.75" customHeight="1">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
+      <c r="A44" s="10" t="s">
+        <v>577</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>580</v>
+      </c>
     </row>
     <row r="45" ht="12.75" customHeight="1">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+      <c r="A45" s="10" t="s">
+        <v>581</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="46" ht="12.75" customHeight="1">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
+      <c r="A46" s="10" t="s">
+        <v>585</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>588</v>
+      </c>
     </row>
     <row r="47" ht="12.75" customHeight="1">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
+      <c r="A47" s="10" t="s">
+        <v>589</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>592</v>
+      </c>
     </row>
     <row r="48" ht="12.75" customHeight="1">
       <c r="A48" s="1"/>

</xml_diff>